<commit_message>
updates for not in Lewis
</commit_message>
<xml_diff>
--- a/input/Lewis World Species List 15 JUNE 2021.xlsx
+++ b/input/Lewis World Species List 15 JUNE 2021.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/18c1f91d246f9ff5/Documents/GitHub/tpt-siphonaptera/input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{9B5E7F5F-8726-4451-ACCF-D0DCAE99AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2AA725D9-2A0C-41E7-8453-2354F5AEEF29}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{9B5E7F5F-8726-4451-ACCF-D0DCAE99AD0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6C18D5D9-62B7-417F-A135-A373CB6BBDEC}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -13087,8 +13087,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H3330"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3170" workbookViewId="0">
-      <selection activeCell="A3170" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A1158" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>